<commit_message>
created a new preprocessing function without loops, and set up a keyword preprocessing comparison notebook. Temptatively restored the original regex preprocessing in both text and keywords.
</commit_message>
<xml_diff>
--- a/keys_update_27012020.xlsx
+++ b/keys_update_27012020.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c0ac04fbadbefb8/SDG/Policy-Mapping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miche\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{6839BC88-B879-4AF7-B057-B7C261F90372}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7D30B152-7FA3-4B50-98DD-BC2E00AF340B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCEBD51-929E-4E24-91BC-8100DC7BE053}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Target_keys" sheetId="1" r:id="rId1"/>
     <sheet name="Goal_keys" sheetId="4" r:id="rId2"/>
     <sheet name="MOI" sheetId="2" r:id="rId3"/>
     <sheet name="developing_countries" sheetId="3" r:id="rId4"/>
-    <sheet name="misc" sheetId="5" r:id="rId5"/>
+    <sheet name="Misc" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2032,11 +2032,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J170"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B122" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="B66" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3790,8 +3790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4006,7 +4006,7 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A11" sqref="A11:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4074,11 +4074,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5029E97-6A1D-4DAE-BD23-6FC994029F3A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865447D5-E220-4502-87A6-A772F08A5B83}">
   <dimension ref="A2:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F8"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finished new preprocessing function, reorganized polmap module, moved old preprocessinf to polmap/deprecated.py, created a keyword comparison notebook, to fix ' ' in keyword_count_polmap
</commit_message>
<xml_diff>
--- a/keys_update_27012020.xlsx
+++ b/keys_update_27012020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miche\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c0ac04fbadbefb8/SDG/Policy-Mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCEBD51-929E-4E24-91BC-8100DC7BE053}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{1DCEBD51-929E-4E24-91BC-8100DC7BE053}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{50D7A86F-E3F5-43B6-9257-A923619D112B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Target_keys" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="468">
   <si>
     <t>1.1</t>
   </si>
@@ -874,9 +874,6 @@
     <t>maternal mortality; death in pregnancy;death in childbirth;maternal deaths;deaths which occur during pregnancy;obstetric deaths;death occurring in childbirth;pregnancy related deaths;pregnancy deaths;deaths related to pregnancy;deaths related to childbirth;MMR;MMRate;maternal health;</t>
   </si>
   <si>
-    <t>hepatitis;malaria;neglected tropical diseases;communicable diseases;water-borne diseases;AIDS;end epidemics;HIV;hivaids;tuberculosis;cope with epidemic;combat pandemic;combat epidemic;combat COVID-19;stem COVID transmission;</t>
-  </si>
-  <si>
     <t>premature mortality;suicide mortality rate;mental health;chronic respiratory disease;cardiovascular disease;diabetes;cancer;non-communicable diseases;ncd;carcinogens;suicide deaths;promote mental health;</t>
   </si>
   <si>
@@ -1003,9 +1000,6 @@
     <t>economic equality;economic inequalities;equitable income growth;equitable distribution of income;equal payment;income equality;income inequality;equal income;payment inequality;payment equality;Inequalities based on income;Gini index;income disparities;distribution of real income;</t>
   </si>
   <si>
-    <t>political inclusion;social inclusion;economic inclusion;social inequalities;political inequalities;Inequalities based on age;Inequalities based on disability;Inequalities based on sexual orientation;Inequalities based on race;Inequalities based on class;Inequalities based on ethnicity;Inequalities based on religion;race inequalities;class inequalities;ethnicity inequalities;religion inequalities;empower lower income earners;people living below 50 per cent of median income;</t>
-  </si>
-  <si>
     <t>inequalities of outcome;discriminatory law;equal opportunity;discrimination;discriminatory practices;equality act;equality of outcome;equal treatment;inequalities of opportunity;disparities of opportunity;be discriminated;racism;homophobia;transphobia;religious intolerance;discriminatory policies;</t>
   </si>
   <si>
@@ -1130,9 +1124,6 @@
   </si>
   <si>
     <t>birth certificate;legal identity;legal registration and documentation of a person;undocumented people;birth registration;registered births;civil registration;children officially recorded;stateless;denied nationality;legally invisible;births were never registered;births not registered;Registration of birth;</t>
-  </si>
-  <si>
-    <t>public access to information;information access;free media;free press;threaten journalist;torture journalist;kidnapping journalist;killing journalist;journalists under risk;human right advocate;disappearances of human rights defenders;disappearances of journalists;disappearances of trade unionists;human rights defenders death;journalists death;trade unionists death;torture of human rights defenders;torture of trade unionists;Freedom to express views;Freedom to express opinion;freedom of information;right to information;</t>
   </si>
   <si>
     <t>capacity building;Paris Principles;prevent violence;combat terrorism;combat crime;prevent crime;fight terrorism;counter terrorism;tackle terrorism;prosecute terrorism;address the threat of terrorist offences;terrorist offences and serious crime;prosecute terrorist offences;human rights institutions;institutions for human rights;NHRI;</t>
@@ -1208,9 +1199,6 @@
     <t>technical skills;vocational skills;skills for employment;digital skills;ICT skills;technology skills;skill training;vocational training; vocational education;upgrading of skills;skills adjusted to labour market;reskilling;upskilling;skills for job;skills for labour market;</t>
   </si>
   <si>
-    <t>numeracy;literacy;language proficiency;underachievement in reading;reading skills;reading proficiency;math proficiency;mathematical proficiency;math skills;mathematical skills;underachiever in mathematics;proficiency standards in reading;proficiency standards in mathematics;reduce illiterate;proficiency in reading;proficiency in math;functionally literate;</t>
-  </si>
-  <si>
     <t>education facilities;safe learning environment;inclusive learning environment;effective learning environment;sanitation in school;electricity in school;internet in school;drinking water in school;schools offering basic services;schools with basic resources;schools with drinking water;schools with electricity;schools with computers;schools with Internet;schools with sanitation;schools with access to electricity;schools with access to Internet;school with basic handwashing facilities;school with handwashing facilities; handwashing facilities in school;internet for teaching;internet accessible by pupils;students can access to internet;internet access students;internet for students;computer for teaching;computer for learning;computer in school;Accessible learning materials;access in schools to key basic services;access in schools to basic services;access in schools to facilities;</t>
   </si>
   <si>
@@ -1440,6 +1428,21 @@
   </si>
   <si>
     <t>SDG 17</t>
+  </si>
+  <si>
+    <t>numeracy;literacy;language proficiency;underachievement in reading;reading skills;reading proficiency;math proficiency;mathematical proficiency;math skills;mathematical skills;underachiever in mathematics;proficiency standards in reading;proficiency standards in mathematics;reduce illiterate;proficiency in reading;proficiency in math;functionally literate;</t>
+  </si>
+  <si>
+    <t>public access to information;information access;free media;free press;threaten journalist;torture journalist;kidnapping journalist;killing journalist;journalists under risk;human right advocate;disappearences of human rights defenders;disappearances of journalists;disappearances of trade unionists;human rights defenders death;journalists death;trade unionists death;torture of human rights defenders;torture of trade unionists;Freedom to express views;Freedom to express opinion;freedom of information;right to information;</t>
+  </si>
+  <si>
+    <t>political inclusion;social inclusion;economic inclusion;social inequalities;political inequalities;Inequalities based on age;Inequalities based on disability;Inequalities based on sexual orientation;Inequalities based on race;Inequalities based on class;Inequalities based on ethnicity;Inequalities based on religion;race inequalities;class inequalities;ethnicity inequalities;religion inequalities;empower lower income earners;people living below 50 perc-ent of median income;</t>
+  </si>
+  <si>
+    <t>hepatitis;malaria;neglected tropical diseases;communicable diseases;water-borne diseases;AIDS;end epidemics;HIV;tuberculosis;cope with epidemic;combat pandemic;combat epidemic;combat COVID-19;stem COVID transmission;</t>
+  </si>
+  <si>
+    <t>hivaids</t>
   </si>
 </sst>
 </file>
@@ -2032,11 +2035,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J170"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B66" sqref="B1:B1048576"/>
+      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2109,7 +2112,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2117,7 +2120,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2125,7 +2128,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2155,7 +2158,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="J9" s="37" t="s">
         <v>262</v>
@@ -2226,7 +2229,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>15</v>
       </c>
@@ -2234,87 +2237,90 @@
         <v>277</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+      <c r="J19" s="37" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>26</v>
       </c>
@@ -2322,36 +2328,36 @@
         <v>204</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>224</v>
@@ -2362,7 +2368,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2370,7 +2376,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>252</v>
@@ -2381,7 +2387,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>389</v>
+        <v>463</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>221</v>
@@ -2392,7 +2398,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>222</v>
@@ -2403,7 +2409,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>223</v>
@@ -2414,7 +2420,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2422,7 +2428,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -2430,7 +2436,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -2438,7 +2444,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -2446,7 +2452,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -2454,7 +2460,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2462,7 +2468,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -2470,7 +2476,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -2478,7 +2484,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -2486,7 +2492,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -2494,7 +2500,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2502,7 +2508,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2510,7 +2516,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2518,7 +2524,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2526,7 +2532,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2534,7 +2540,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2542,7 +2548,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2550,7 +2556,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2558,7 +2564,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2566,7 +2572,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2574,7 +2580,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2582,7 +2588,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2590,7 +2596,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2598,7 +2604,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2606,7 +2612,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2614,7 +2620,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2622,7 +2628,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
@@ -2630,7 +2636,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
@@ -2638,7 +2644,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -2646,7 +2652,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -2654,7 +2660,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -2662,7 +2668,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
@@ -2670,7 +2676,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
@@ -2678,7 +2684,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
@@ -2686,7 +2692,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
@@ -2694,7 +2700,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -2702,7 +2708,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -2710,7 +2716,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
@@ -2718,7 +2724,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
@@ -2726,10 +2732,10 @@
         <v>75</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J77" s="34" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
@@ -2737,7 +2743,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -2745,10 +2751,10 @@
         <v>77</v>
       </c>
       <c r="B79" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="J79" s="34" t="s">
         <v>316</v>
-      </c>
-      <c r="J79" s="34" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
@@ -2756,7 +2762,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -2764,7 +2770,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -2772,7 +2778,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C82" s="15" t="s">
         <v>229</v>
@@ -2783,7 +2789,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>321</v>
+        <v>465</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -2791,7 +2797,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -2799,7 +2805,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -2807,7 +2813,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -2815,7 +2821,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C87" s="15" t="s">
         <v>230</v>
@@ -2826,7 +2832,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C88" s="15" t="s">
         <v>231</v>
@@ -2837,7 +2843,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C89" s="15" t="s">
         <v>232</v>
@@ -2848,7 +2854,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -2856,7 +2862,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -2864,7 +2870,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -2872,7 +2878,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -2880,7 +2886,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -2888,7 +2894,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -2896,7 +2902,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
@@ -2904,7 +2910,7 @@
         <v>95</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
@@ -2912,7 +2918,7 @@
         <v>96</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
@@ -2920,7 +2926,7 @@
         <v>97</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
@@ -2928,7 +2934,7 @@
         <v>98</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
@@ -2944,7 +2950,7 @@
         <v>100</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
@@ -2952,7 +2958,7 @@
         <v>101</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C103" s="15" t="s">
         <v>236</v>
@@ -2963,7 +2969,7 @@
         <v>102</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
@@ -2971,7 +2977,7 @@
         <v>103</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="106" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2995,7 +3001,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
@@ -3011,7 +3017,7 @@
         <v>107</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="C109" s="15" t="s">
         <v>237</v>
@@ -3033,7 +3039,7 @@
         <v>109</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
@@ -3049,7 +3055,7 @@
         <v>111</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -3057,7 +3063,7 @@
         <v>112</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -3065,7 +3071,7 @@
         <v>113</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -3073,7 +3079,7 @@
         <v>114</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -3081,7 +3087,7 @@
         <v>115</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -3089,7 +3095,7 @@
         <v>116</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -3097,7 +3103,7 @@
         <v>117</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -3105,7 +3111,7 @@
         <v>118</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -3113,7 +3119,7 @@
         <v>119</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -3121,7 +3127,7 @@
         <v>120</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -3129,7 +3135,7 @@
         <v>121</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -3137,7 +3143,7 @@
         <v>122</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -3145,7 +3151,7 @@
         <v>123</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -3153,7 +3159,7 @@
         <v>124</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -3161,7 +3167,7 @@
         <v>125</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -3169,7 +3175,7 @@
         <v>126</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3177,7 +3183,7 @@
         <v>127</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C129" s="15" t="s">
         <v>244</v>
@@ -3188,7 +3194,7 @@
         <v>128</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C130" s="15" t="s">
         <v>245</v>
@@ -3199,7 +3205,7 @@
         <v>129</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C131" s="15" t="s">
         <v>246</v>
@@ -3210,7 +3216,7 @@
         <v>130</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C132" s="15" t="s">
         <v>247</v>
@@ -3221,7 +3227,7 @@
         <v>131</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C133" s="15" t="s">
         <v>248</v>
@@ -3243,7 +3249,7 @@
         <v>133</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -3251,7 +3257,7 @@
         <v>134</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C136" s="15" t="s">
         <v>241</v>
@@ -3262,7 +3268,7 @@
         <v>135</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C137" s="15" t="s">
         <v>249</v>
@@ -3273,13 +3279,13 @@
         <v>136</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="C138" s="15" t="s">
         <v>250</v>
       </c>
       <c r="D138" s="12" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3287,7 +3293,7 @@
         <v>137</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C139" s="15" t="s">
         <v>251</v>
@@ -3298,7 +3304,7 @@
         <v>138</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3306,7 +3312,7 @@
         <v>139</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -3314,7 +3320,7 @@
         <v>140</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3338,7 +3344,7 @@
         <v>143</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
@@ -3346,7 +3352,7 @@
         <v>144</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
@@ -3354,7 +3360,7 @@
         <v>145</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
@@ -3362,7 +3368,7 @@
         <v>146</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
@@ -3370,7 +3376,7 @@
         <v>147</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>364</v>
+        <v>464</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
@@ -3378,7 +3384,7 @@
         <v>148</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
@@ -3386,7 +3392,7 @@
         <v>149</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
@@ -3394,7 +3400,7 @@
         <v>150</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
@@ -3402,7 +3408,7 @@
         <v>151</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I153" s="38"/>
     </row>
@@ -3411,7 +3417,7 @@
         <v>152</v>
       </c>
       <c r="B154" s="11" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="C154" s="15"/>
       <c r="D154" s="12"/>
@@ -3427,7 +3433,7 @@
         <v>153</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
@@ -3435,7 +3441,7 @@
         <v>154</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
@@ -3443,7 +3449,7 @@
         <v>155</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
@@ -3451,7 +3457,7 @@
         <v>156</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
@@ -3459,7 +3465,7 @@
         <v>157</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
@@ -3467,7 +3473,7 @@
         <v>158</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -3475,7 +3481,7 @@
         <v>159</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -3483,7 +3489,7 @@
         <v>160</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -3491,7 +3497,7 @@
         <v>161</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -3499,7 +3505,7 @@
         <v>162</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -3507,7 +3513,7 @@
         <v>163</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -3515,7 +3521,7 @@
         <v>164</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -3523,7 +3529,7 @@
         <v>165</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -3531,7 +3537,7 @@
         <v>166</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -3539,7 +3545,7 @@
         <v>167</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -3547,7 +3553,7 @@
         <v>168</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -3611,10 +3617,10 @@
     </row>
     <row r="2" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C2" s="25" t="s">
         <v>215</v>
@@ -3628,10 +3634,10 @@
     </row>
     <row r="3" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="L3" s="30" t="s">
         <v>227</v>
@@ -3640,10 +3646,10 @@
     </row>
     <row r="4" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="28" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>239</v>
@@ -3651,10 +3657,10 @@
     </row>
     <row r="5" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>220</v>
@@ -3662,10 +3668,10 @@
     </row>
     <row r="6" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>234</v>
@@ -3673,42 +3679,42 @@
     </row>
     <row r="7" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="28" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="28" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="28" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="28" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>233</v>
@@ -3716,18 +3722,18 @@
     </row>
     <row r="12" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="28" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="28" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>238</v>
@@ -3735,26 +3741,26 @@
     </row>
     <row r="14" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="28" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="28" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>242</v>
@@ -3762,10 +3768,10 @@
     </row>
     <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>240</v>
@@ -3773,10 +3779,10 @@
     </row>
     <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="28" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -3790,7 +3796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -3887,7 +3893,7 @@
         <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3928,7 +3934,7 @@
         <v>153</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3936,7 +3942,7 @@
         <v>154</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3944,7 +3950,7 @@
         <v>156</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>